<commit_message>
Finished function for generating full database
</commit_message>
<xml_diff>
--- a/country_codes_independence_status.xlsx
+++ b/country_codes_independence_status.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Diogo\Profissional\Bootcamp ENAP\Modulo 2 - Ciências de Dados\projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Diogo\Profissional\Bootcamp ENAP\Modulo 2 - Ciências de Dados\gdp_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1C01FE-9941-4F5C-82E5-0A229204F333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA606DA-F777-4015-A863-B3762B35DCA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3732" yWindow="3732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="507">
   <si>
     <t>Alpha-3 code</t>
   </si>
@@ -1545,7 +1545,10 @@
     <t>Present in Scimago databse</t>
   </si>
   <si>
-    <t>Tax haven?</t>
+    <t>Conduit OFC</t>
+  </si>
+  <si>
+    <t>Sink OFC</t>
   </si>
 </sst>
 </file>
@@ -1908,8 +1911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F228" sqref="F228"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1918,6 +1921,7 @@
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="5.77734375" customWidth="1"/>
     <col min="4" max="4" width="5.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
     <col min="8" max="8" width="33.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1935,6 +1939,9 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>506</v>
+      </c>
+      <c r="F1" t="s">
         <v>505</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -1955,6 +1962,9 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1974,6 +1984,9 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -1991,6 +2004,9 @@
       <c r="E4" t="s">
         <v>6</v>
       </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -2008,6 +2024,9 @@
       <c r="E5" t="s">
         <v>6</v>
       </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -2025,6 +2044,9 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -2042,6 +2064,9 @@
       <c r="E7" t="s">
         <v>4</v>
       </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -2059,6 +2084,9 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -2076,6 +2104,9 @@
       <c r="E9" t="s">
         <v>4</v>
       </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -2093,6 +2124,9 @@
       <c r="E10" t="s">
         <v>6</v>
       </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -2110,6 +2144,9 @@
       <c r="E11" t="s">
         <v>4</v>
       </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -2127,6 +2164,9 @@
       <c r="E12" t="s">
         <v>6</v>
       </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -2144,6 +2184,9 @@
       <c r="E13" t="s">
         <v>6</v>
       </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -2161,6 +2204,9 @@
       <c r="E14" t="s">
         <v>4</v>
       </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -2178,6 +2224,9 @@
       <c r="E15" t="s">
         <v>6</v>
       </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -2195,8 +2244,11 @@
       <c r="E16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>31</v>
       </c>
@@ -2212,8 +2264,11 @@
       <c r="E17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>44</v>
       </c>
@@ -2229,8 +2284,11 @@
       <c r="E18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>48</v>
       </c>
@@ -2246,8 +2304,11 @@
       <c r="E19" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>50</v>
       </c>
@@ -2263,8 +2324,11 @@
       <c r="E20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>52</v>
       </c>
@@ -2280,8 +2344,11 @@
       <c r="E21" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>112</v>
       </c>
@@ -2297,8 +2364,11 @@
       <c r="E22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>56</v>
       </c>
@@ -2314,8 +2384,11 @@
       <c r="E23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>84</v>
       </c>
@@ -2331,8 +2404,11 @@
       <c r="E24" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>204</v>
       </c>
@@ -2348,8 +2424,11 @@
       <c r="E25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>60</v>
       </c>
@@ -2365,8 +2444,11 @@
       <c r="E26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>64</v>
       </c>
@@ -2382,8 +2464,11 @@
       <c r="E27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>68</v>
       </c>
@@ -2399,8 +2484,11 @@
       <c r="E28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>535</v>
       </c>
@@ -2416,8 +2504,11 @@
       <c r="E29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>70</v>
       </c>
@@ -2433,8 +2524,11 @@
       <c r="E30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>72</v>
       </c>
@@ -2450,8 +2544,11 @@
       <c r="E31" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>74</v>
       </c>
@@ -2467,8 +2564,11 @@
       <c r="E32" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>76</v>
       </c>
@@ -2484,8 +2584,11 @@
       <c r="E33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>86</v>
       </c>
@@ -2501,8 +2604,11 @@
       <c r="E34" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>96</v>
       </c>
@@ -2518,8 +2624,11 @@
       <c r="E35" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>100</v>
       </c>
@@ -2535,8 +2644,11 @@
       <c r="E36" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>854</v>
       </c>
@@ -2552,8 +2664,11 @@
       <c r="E37" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>108</v>
       </c>
@@ -2569,8 +2684,11 @@
       <c r="E38" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>132</v>
       </c>
@@ -2586,8 +2704,11 @@
       <c r="E39" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>116</v>
       </c>
@@ -2603,8 +2724,11 @@
       <c r="E40" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>120</v>
       </c>
@@ -2620,8 +2744,11 @@
       <c r="E41" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>124</v>
       </c>
@@ -2637,8 +2764,11 @@
       <c r="E42" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>136</v>
       </c>
@@ -2654,8 +2784,11 @@
       <c r="E43" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>140</v>
       </c>
@@ -2671,8 +2804,11 @@
       <c r="E44" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>148</v>
       </c>
@@ -2688,8 +2824,11 @@
       <c r="E45" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>152</v>
       </c>
@@ -2705,8 +2844,11 @@
       <c r="E46" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>156</v>
       </c>
@@ -2722,8 +2864,11 @@
       <c r="E47" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>162</v>
       </c>
@@ -2739,8 +2884,11 @@
       <c r="E48" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>166</v>
       </c>
@@ -2756,8 +2904,11 @@
       <c r="E49" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>170</v>
       </c>
@@ -2773,8 +2924,11 @@
       <c r="E50" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>174</v>
       </c>
@@ -2790,8 +2944,11 @@
       <c r="E51" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>178</v>
       </c>
@@ -2807,8 +2964,11 @@
       <c r="E52" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>180</v>
       </c>
@@ -2824,8 +2984,11 @@
       <c r="E53" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>184</v>
       </c>
@@ -2841,8 +3004,11 @@
       <c r="E54" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>188</v>
       </c>
@@ -2858,8 +3024,11 @@
       <c r="E55" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>384</v>
       </c>
@@ -2875,8 +3044,11 @@
       <c r="E56" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>191</v>
       </c>
@@ -2892,8 +3064,11 @@
       <c r="E57" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>192</v>
       </c>
@@ -2909,8 +3084,11 @@
       <c r="E58" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>531</v>
       </c>
@@ -2926,8 +3104,11 @@
       <c r="E59" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>196</v>
       </c>
@@ -2943,8 +3124,11 @@
       <c r="E60" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>203</v>
       </c>
@@ -2960,8 +3144,11 @@
       <c r="E61" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>208</v>
       </c>
@@ -2977,8 +3164,11 @@
       <c r="E62" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>262</v>
       </c>
@@ -2994,8 +3184,11 @@
       <c r="E63" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>212</v>
       </c>
@@ -3011,8 +3204,11 @@
       <c r="E64" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>214</v>
       </c>
@@ -3028,8 +3224,11 @@
       <c r="E65" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>218</v>
       </c>
@@ -3045,8 +3244,11 @@
       <c r="E66" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>818</v>
       </c>
@@ -3062,8 +3264,11 @@
       <c r="E67" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>222</v>
       </c>
@@ -3079,8 +3284,11 @@
       <c r="E68" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>226</v>
       </c>
@@ -3096,8 +3304,11 @@
       <c r="E69" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>232</v>
       </c>
@@ -3113,8 +3324,11 @@
       <c r="E70" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>233</v>
       </c>
@@ -3130,8 +3344,11 @@
       <c r="E71" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>748</v>
       </c>
@@ -3147,8 +3364,11 @@
       <c r="E72" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>231</v>
       </c>
@@ -3164,8 +3384,11 @@
       <c r="E73" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>238</v>
       </c>
@@ -3181,8 +3404,11 @@
       <c r="E74" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>234</v>
       </c>
@@ -3198,8 +3424,11 @@
       <c r="E75" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>242</v>
       </c>
@@ -3215,8 +3444,11 @@
       <c r="E76" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>246</v>
       </c>
@@ -3232,8 +3464,11 @@
       <c r="E77" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>250</v>
       </c>
@@ -3249,8 +3484,11 @@
       <c r="E78" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>254</v>
       </c>
@@ -3266,8 +3504,11 @@
       <c r="E79" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>258</v>
       </c>
@@ -3283,8 +3524,11 @@
       <c r="E80" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>260</v>
       </c>
@@ -3300,8 +3544,11 @@
       <c r="E81" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>266</v>
       </c>
@@ -3317,8 +3564,11 @@
       <c r="E82" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>270</v>
       </c>
@@ -3334,8 +3584,11 @@
       <c r="E83" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>268</v>
       </c>
@@ -3351,8 +3604,11 @@
       <c r="E84" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>276</v>
       </c>
@@ -3368,8 +3624,11 @@
       <c r="E85" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>288</v>
       </c>
@@ -3385,8 +3644,11 @@
       <c r="E86" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>292</v>
       </c>
@@ -3402,8 +3664,11 @@
       <c r="E87" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>300</v>
       </c>
@@ -3419,8 +3684,11 @@
       <c r="E88" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F88" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>304</v>
       </c>
@@ -3436,8 +3704,11 @@
       <c r="E89" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F89" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>308</v>
       </c>
@@ -3453,8 +3724,11 @@
       <c r="E90" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>312</v>
       </c>
@@ -3470,8 +3744,11 @@
       <c r="E91" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>316</v>
       </c>
@@ -3487,8 +3764,11 @@
       <c r="E92" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F92" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>320</v>
       </c>
@@ -3504,8 +3784,11 @@
       <c r="E93" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F93" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>831</v>
       </c>
@@ -3521,8 +3804,11 @@
       <c r="E94" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>324</v>
       </c>
@@ -3538,8 +3824,11 @@
       <c r="E95" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>624</v>
       </c>
@@ -3555,8 +3844,11 @@
       <c r="E96" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>328</v>
       </c>
@@ -3572,8 +3864,11 @@
       <c r="E97" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>332</v>
       </c>
@@ -3589,8 +3884,11 @@
       <c r="E98" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>334</v>
       </c>
@@ -3606,8 +3904,11 @@
       <c r="E99" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>336</v>
       </c>
@@ -3623,8 +3924,11 @@
       <c r="E100" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F100" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>340</v>
       </c>
@@ -3640,8 +3944,11 @@
       <c r="E101" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F101" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>344</v>
       </c>
@@ -3657,8 +3964,11 @@
       <c r="E102" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>348</v>
       </c>
@@ -3674,8 +3984,11 @@
       <c r="E103" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>352</v>
       </c>
@@ -3691,8 +4004,11 @@
       <c r="E104" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>356</v>
       </c>
@@ -3708,8 +4024,11 @@
       <c r="E105" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>360</v>
       </c>
@@ -3725,8 +4044,11 @@
       <c r="E106" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F106" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>364</v>
       </c>
@@ -3742,8 +4064,11 @@
       <c r="E107" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>368</v>
       </c>
@@ -3759,8 +4084,11 @@
       <c r="E108" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>372</v>
       </c>
@@ -3774,10 +4102,13 @@
         <v>112</v>
       </c>
       <c r="E109" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F109" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>833</v>
       </c>
@@ -3793,8 +4124,11 @@
       <c r="E110" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F110" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>376</v>
       </c>
@@ -3810,8 +4144,11 @@
       <c r="E111" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>380</v>
       </c>
@@ -3827,8 +4164,11 @@
       <c r="E112" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>388</v>
       </c>
@@ -3844,8 +4184,11 @@
       <c r="E113" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F113" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>392</v>
       </c>
@@ -3861,8 +4204,11 @@
       <c r="E114" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F114" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>832</v>
       </c>
@@ -3878,8 +4224,11 @@
       <c r="E115" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F115" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>400</v>
       </c>
@@ -3895,8 +4244,11 @@
       <c r="E116" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F116" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>398</v>
       </c>
@@ -3912,8 +4264,11 @@
       <c r="E117" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F117" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>404</v>
       </c>
@@ -3929,8 +4284,11 @@
       <c r="E118" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>296</v>
       </c>
@@ -3946,8 +4304,11 @@
       <c r="E119" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F119" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>408</v>
       </c>
@@ -3963,8 +4324,11 @@
       <c r="E120" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F120" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>410</v>
       </c>
@@ -3980,8 +4344,11 @@
       <c r="E121" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F121" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>414</v>
       </c>
@@ -3997,8 +4364,11 @@
       <c r="E122" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F122" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>417</v>
       </c>
@@ -4014,8 +4384,11 @@
       <c r="E123" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F123" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>418</v>
       </c>
@@ -4031,8 +4404,11 @@
       <c r="E124" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F124" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>428</v>
       </c>
@@ -4048,8 +4424,11 @@
       <c r="E125" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F125" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>422</v>
       </c>
@@ -4065,8 +4444,11 @@
       <c r="E126" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F126" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>426</v>
       </c>
@@ -4082,8 +4464,11 @@
       <c r="E127" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F127" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>430</v>
       </c>
@@ -4099,8 +4484,11 @@
       <c r="E128" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F128" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>434</v>
       </c>
@@ -4116,8 +4504,11 @@
       <c r="E129" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>438</v>
       </c>
@@ -4133,8 +4524,11 @@
       <c r="E130" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F130" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>440</v>
       </c>
@@ -4150,8 +4544,11 @@
       <c r="E131" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F131" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>442</v>
       </c>
@@ -4167,8 +4564,11 @@
       <c r="E132" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F132" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>446</v>
       </c>
@@ -4184,8 +4584,11 @@
       <c r="E133" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F133" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>450</v>
       </c>
@@ -4201,8 +4604,11 @@
       <c r="E134" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F134" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>454</v>
       </c>
@@ -4218,8 +4624,11 @@
       <c r="E135" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F135" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>458</v>
       </c>
@@ -4235,8 +4644,11 @@
       <c r="E136" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F136" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>462</v>
       </c>
@@ -4252,8 +4664,11 @@
       <c r="E137" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F137" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>466</v>
       </c>
@@ -4269,8 +4684,11 @@
       <c r="E138" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F138" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>470</v>
       </c>
@@ -4286,8 +4704,11 @@
       <c r="E139" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F139" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>584</v>
       </c>
@@ -4303,8 +4724,11 @@
       <c r="E140" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F140" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>474</v>
       </c>
@@ -4320,8 +4744,11 @@
       <c r="E141" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F141" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>478</v>
       </c>
@@ -4337,8 +4764,11 @@
       <c r="E142" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F142" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>480</v>
       </c>
@@ -4354,8 +4784,11 @@
       <c r="E143" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F143" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>175</v>
       </c>
@@ -4371,8 +4804,11 @@
       <c r="E144" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F144" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>484</v>
       </c>
@@ -4388,8 +4824,11 @@
       <c r="E145" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F145" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>583</v>
       </c>
@@ -4405,8 +4844,11 @@
       <c r="E146" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F146" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>498</v>
       </c>
@@ -4422,8 +4864,11 @@
       <c r="E147" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F147" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>492</v>
       </c>
@@ -4439,8 +4884,11 @@
       <c r="E148" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F148" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>496</v>
       </c>
@@ -4456,8 +4904,11 @@
       <c r="E149" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F149" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>499</v>
       </c>
@@ -4473,8 +4924,11 @@
       <c r="E150" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F150" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>500</v>
       </c>
@@ -4490,8 +4944,11 @@
       <c r="E151" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F151" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>504</v>
       </c>
@@ -4507,8 +4964,11 @@
       <c r="E152" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F152" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>508</v>
       </c>
@@ -4524,8 +4984,11 @@
       <c r="E153" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F153" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>104</v>
       </c>
@@ -4541,8 +5004,11 @@
       <c r="E154" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F154" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>516</v>
       </c>
@@ -4558,8 +5024,11 @@
       <c r="E155" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F155" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>520</v>
       </c>
@@ -4575,8 +5044,11 @@
       <c r="E156" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F156" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>524</v>
       </c>
@@ -4592,8 +5064,11 @@
       <c r="E157" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F157" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>528</v>
       </c>
@@ -4607,10 +5082,13 @@
         <v>161</v>
       </c>
       <c r="E158" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F158" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>540</v>
       </c>
@@ -4626,8 +5104,11 @@
       <c r="E159" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F159" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>554</v>
       </c>
@@ -4643,8 +5124,11 @@
       <c r="E160" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F160" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>558</v>
       </c>
@@ -4660,8 +5144,11 @@
       <c r="E161" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F161" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>562</v>
       </c>
@@ -4677,8 +5164,11 @@
       <c r="E162" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F162" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>566</v>
       </c>
@@ -4694,8 +5184,11 @@
       <c r="E163" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F163" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>570</v>
       </c>
@@ -4711,8 +5204,11 @@
       <c r="E164" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F164" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>574</v>
       </c>
@@ -4728,8 +5224,11 @@
       <c r="E165" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F165" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>807</v>
       </c>
@@ -4745,8 +5244,11 @@
       <c r="E166" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F166" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>580</v>
       </c>
@@ -4762,8 +5264,11 @@
       <c r="E167" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F167" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>578</v>
       </c>
@@ -4779,8 +5284,11 @@
       <c r="E168" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F168" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>512</v>
       </c>
@@ -4796,8 +5304,11 @@
       <c r="E169" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F169" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>586</v>
       </c>
@@ -4813,8 +5324,11 @@
       <c r="E170" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F170" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>585</v>
       </c>
@@ -4830,8 +5344,11 @@
       <c r="E171" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F171" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>275</v>
       </c>
@@ -4847,8 +5364,11 @@
       <c r="E172" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F172" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>591</v>
       </c>
@@ -4864,8 +5384,11 @@
       <c r="E173" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F173" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>598</v>
       </c>
@@ -4881,8 +5404,11 @@
       <c r="E174" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F174" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>600</v>
       </c>
@@ -4898,8 +5424,11 @@
       <c r="E175" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F175" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>604</v>
       </c>
@@ -4915,8 +5444,11 @@
       <c r="E176" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F176" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>608</v>
       </c>
@@ -4932,8 +5464,11 @@
       <c r="E177" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F177" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>612</v>
       </c>
@@ -4949,8 +5484,11 @@
       <c r="E178" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F178" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>616</v>
       </c>
@@ -4966,8 +5504,11 @@
       <c r="E179" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F179" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>620</v>
       </c>
@@ -4983,8 +5524,11 @@
       <c r="E180" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F180" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>630</v>
       </c>
@@ -5000,8 +5544,11 @@
       <c r="E181" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F181" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>634</v>
       </c>
@@ -5017,8 +5564,11 @@
       <c r="E182" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F182" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>638</v>
       </c>
@@ -5034,8 +5584,11 @@
       <c r="E183" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F183" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>642</v>
       </c>
@@ -5051,8 +5604,11 @@
       <c r="E184" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F184" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>643</v>
       </c>
@@ -5068,8 +5624,11 @@
       <c r="E185" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F185" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>646</v>
       </c>
@@ -5085,8 +5644,11 @@
       <c r="E186" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F186" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>652</v>
       </c>
@@ -5102,8 +5664,11 @@
       <c r="E187" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F187" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>654</v>
       </c>
@@ -5119,8 +5684,11 @@
       <c r="E188" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F188" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>659</v>
       </c>
@@ -5136,8 +5704,11 @@
       <c r="E189" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F189" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>662</v>
       </c>
@@ -5153,8 +5724,11 @@
       <c r="E190" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F190" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>663</v>
       </c>
@@ -5170,8 +5744,11 @@
       <c r="E191" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F191" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>666</v>
       </c>
@@ -5187,8 +5764,11 @@
       <c r="E192" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F192" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>670</v>
       </c>
@@ -5204,8 +5784,11 @@
       <c r="E193" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F193" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>882</v>
       </c>
@@ -5221,8 +5804,11 @@
       <c r="E194" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F194" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>674</v>
       </c>
@@ -5238,8 +5824,11 @@
       <c r="E195" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F195" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>678</v>
       </c>
@@ -5255,8 +5844,11 @@
       <c r="E196" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F196" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>682</v>
       </c>
@@ -5272,8 +5864,11 @@
       <c r="E197" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F197" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>686</v>
       </c>
@@ -5289,8 +5884,11 @@
       <c r="E198" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F198" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>688</v>
       </c>
@@ -5306,8 +5904,11 @@
       <c r="E199" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F199" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>690</v>
       </c>
@@ -5323,8 +5924,11 @@
       <c r="E200" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F200" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>694</v>
       </c>
@@ -5340,8 +5944,11 @@
       <c r="E201" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F201" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>702</v>
       </c>
@@ -5355,10 +5962,13 @@
         <v>205</v>
       </c>
       <c r="E202" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F202" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>534</v>
       </c>
@@ -5374,8 +5984,11 @@
       <c r="E203" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F203" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>703</v>
       </c>
@@ -5391,8 +6004,11 @@
       <c r="E204" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F204" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>705</v>
       </c>
@@ -5408,8 +6024,11 @@
       <c r="E205" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F205" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>90</v>
       </c>
@@ -5425,8 +6044,11 @@
       <c r="E206" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F206" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>706</v>
       </c>
@@ -5442,8 +6064,11 @@
       <c r="E207" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F207" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>710</v>
       </c>
@@ -5459,8 +6084,11 @@
       <c r="E208" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F208" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>239</v>
       </c>
@@ -5476,8 +6104,11 @@
       <c r="E209" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F209" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>728</v>
       </c>
@@ -5493,8 +6124,11 @@
       <c r="E210" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F210" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>724</v>
       </c>
@@ -5510,8 +6144,11 @@
       <c r="E211" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F211" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>144</v>
       </c>
@@ -5527,8 +6164,11 @@
       <c r="E212" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F212" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>729</v>
       </c>
@@ -5544,8 +6184,11 @@
       <c r="E213" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F213" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>740</v>
       </c>
@@ -5561,8 +6204,11 @@
       <c r="E214" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F214" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>744</v>
       </c>
@@ -5578,8 +6224,11 @@
       <c r="E215" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F215" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>752</v>
       </c>
@@ -5595,8 +6244,11 @@
       <c r="E216" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F216" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>756</v>
       </c>
@@ -5610,10 +6262,13 @@
         <v>220</v>
       </c>
       <c r="E217" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F217" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>760</v>
       </c>
@@ -5629,8 +6284,11 @@
       <c r="E218" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F218" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>158</v>
       </c>
@@ -5646,8 +6304,11 @@
       <c r="E219" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F219" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>762</v>
       </c>
@@ -5663,8 +6324,11 @@
       <c r="E220" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F220" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>834</v>
       </c>
@@ -5680,8 +6344,11 @@
       <c r="E221" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F221" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>764</v>
       </c>
@@ -5697,8 +6364,11 @@
       <c r="E222" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F222" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>626</v>
       </c>
@@ -5714,8 +6384,11 @@
       <c r="E223" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F223" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>768</v>
       </c>
@@ -5731,8 +6404,11 @@
       <c r="E224" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F224" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>772</v>
       </c>
@@ -5748,8 +6424,11 @@
       <c r="E225" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F225" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>776</v>
       </c>
@@ -5765,8 +6444,11 @@
       <c r="E226" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F226" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>780</v>
       </c>
@@ -5782,8 +6464,11 @@
       <c r="E227" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F227" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>788</v>
       </c>
@@ -5799,8 +6484,11 @@
       <c r="E228" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F228" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>792</v>
       </c>
@@ -5816,8 +6504,11 @@
       <c r="E229" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F229" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>795</v>
       </c>
@@ -5833,8 +6524,11 @@
       <c r="E230" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F230" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>796</v>
       </c>
@@ -5850,8 +6544,11 @@
       <c r="E231" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F231" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>798</v>
       </c>
@@ -5867,8 +6564,11 @@
       <c r="E232" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F232" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>800</v>
       </c>
@@ -5884,8 +6584,11 @@
       <c r="E233" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F233" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>804</v>
       </c>
@@ -5901,8 +6604,11 @@
       <c r="E234" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F234" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>784</v>
       </c>
@@ -5918,8 +6624,11 @@
       <c r="E235" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F235" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>826</v>
       </c>
@@ -5933,10 +6642,13 @@
         <v>239</v>
       </c>
       <c r="E236" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F236" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>840</v>
       </c>
@@ -5952,8 +6664,11 @@
       <c r="E237" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F237" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>581</v>
       </c>
@@ -5969,8 +6684,11 @@
       <c r="E238" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F238" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>858</v>
       </c>
@@ -5986,8 +6704,11 @@
       <c r="E239" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F239" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>860</v>
       </c>
@@ -6003,8 +6724,11 @@
       <c r="E240" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F240" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>548</v>
       </c>
@@ -6020,8 +6744,11 @@
       <c r="E241" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F241" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>862</v>
       </c>
@@ -6037,8 +6764,11 @@
       <c r="E242" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F242" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>704</v>
       </c>
@@ -6054,8 +6784,11 @@
       <c r="E243" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F243" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>92</v>
       </c>
@@ -6071,8 +6804,11 @@
       <c r="E244" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F244" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>850</v>
       </c>
@@ -6088,8 +6824,11 @@
       <c r="E245" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F245" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>876</v>
       </c>
@@ -6105,8 +6844,11 @@
       <c r="E246" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F246" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>732</v>
       </c>
@@ -6122,8 +6864,11 @@
       <c r="E247" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F247" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>887</v>
       </c>
@@ -6139,8 +6884,11 @@
       <c r="E248" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F248" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>894</v>
       </c>
@@ -6156,8 +6904,11 @@
       <c r="E249" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F249" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>716</v>
       </c>
@@ -6171,6 +6922,9 @@
         <v>253</v>
       </c>
       <c r="E250" t="s">
+        <v>6</v>
+      </c>
+      <c r="F250" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>